<commit_message>
Modified sheet of problems
</commit_message>
<xml_diff>
--- a/Leet_Coding/LeetCode_to_revisit.xlsx
+++ b/Leet_Coding/LeetCode_to_revisit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aghatnekar\DEVP\Self_Practice\competitive-programming\Leet_Coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEF815C-CCDF-46CA-82B7-BEB0BE38CF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07186A88-0010-4E4B-A66D-EC9EE5C14ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2430" windowWidth="29040" windowHeight="15840" xr2:uid="{151E93C1-2929-4C43-AC3B-99335C268DE9}"/>
   </bookViews>
@@ -445,7 +445,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1C441E-AF6E-488F-B6E7-EAB07CF23E56}">
   <dimension ref="A1:C96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -871,68 +871,68 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="4">
+      <c r="B11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="4">
+      <c r="B12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="1">
+      <c r="B13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="B14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="4">
+      <c r="B15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="4">
+      <c r="B16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="3">
         <v>1</v>
       </c>
     </row>
@@ -944,39 +944,39 @@
         <v>63</v>
       </c>
       <c r="C17" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="4">
+      <c r="B18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="1">
+      <c r="B19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="1">
+      <c r="B20" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="4">
         <v>1</v>
       </c>
     </row>
@@ -1223,35 +1223,35 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C44" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C45" s="3">
         <v>3</v>
       </c>
     </row>
@@ -1322,68 +1322,68 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B52" s="1" t="s">
+      <c r="A52" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C53" s="4">
+      <c r="C53" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C54" s="4">
+      <c r="C54" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C57" s="4">
+      <c r="C57" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1553,101 +1553,101 @@
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" s="4" t="s">
+      <c r="A73" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C73" s="4">
+      <c r="C73" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" s="7" t="s">
+      <c r="A74" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B74" s="7" t="s">
+      <c r="B74" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C74" s="7">
+      <c r="C74" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A76" s="1" t="s">
+      <c r="A76" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" s="1" t="s">
+      <c r="A78" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" s="1" t="s">
+      <c r="A79" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C79" s="1">
+      <c r="C79" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A80" s="1" t="s">
+      <c r="A80" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C80" s="1">
+      <c r="C80" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" s="4" t="s">
+      <c r="A81" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C81" s="4">
+      <c r="C81" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1658,7 +1658,7 @@
       <c r="B82" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1669,84 +1669,84 @@
       <c r="B83" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C83" s="1">
+      <c r="C83" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" s="1" t="s">
+      <c r="A84" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C84" s="1">
+      <c r="C84" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" s="4" t="s">
+      <c r="A85" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C85" s="4">
+      <c r="C85" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" s="1" t="s">
+      <c r="A86" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C86" s="1">
+      <c r="C86" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" s="1" t="s">
+      <c r="A87" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" s="1" t="s">
+      <c r="A88" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C88" s="1">
+      <c r="C88" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A89" s="4" t="s">
+      <c r="A89" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C89" s="4">
+      <c r="C89" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" s="4" t="s">
+      <c r="A90" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B90" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C90" s="4">
+      <c r="C90" s="3">
         <v>3</v>
       </c>
     </row>

</xml_diff>